<commit_message>
feat: Update output file with new timestamp and refresh binary files for consistency
</commit_message>
<xml_diff>
--- a/data/ORÇAMENTO - ACIONAMENTO 01 - REV 05 final.xlsx
+++ b/data/ORÇAMENTO - ACIONAMENTO 01 - REV 05 final.xlsx
@@ -5547,7 +5547,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="314">
   <si>
     <t xml:space="preserve">RESUMO</t>
   </si>
@@ -5985,7 +5985,7 @@
     <t xml:space="preserve"> 100251 </t>
   </si>
   <si>
-    <t xml:space="preserve">Teste TRANSPORTE HORIZONTAL MANUAL, DE TUBO DE AÇO CARBONO LEVE OU MÉDIO, PRETO OU GALVANIZADO, COM DIÂMETRO MAIOR QUE 32 MM E MENOR OU IGUAL A 65 MM (UNIDADE: MXKM). AF_07/2019</t>
+    <t xml:space="preserve">TRANSPORTE HORIZONTAL MANUAL, DE TUBO DE AÇO CARBONO LEVE OU MÉDIO, PRETO OU GALVANIZADO, COM DIÂMETRO MAIOR QUE 32 MM E MENOR OU IGUAL A 65 MM (UNIDADE: MXKM). AF_07/2019</t>
   </si>
   <si>
     <t xml:space="preserve">Transporte de Materiais dentro do Canteiro de Obras</t>
@@ -6178,9 +6178,6 @@
   </si>
   <si>
     <t xml:space="preserve">EPI - FAMILIA SERVENTE - HORISTA (ENCARGOS COMPLEMENTARES - COLETADO CAIXA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSPORTE HORIZONTAL MANUAL, DE TUBO DE AÇO CARBONO LEVE OU MÉDIO, PRETO OU GALVANIZADO, COM DIÂMETRO MAIOR QUE 32 MM E MENOR OU IGUAL A 65 MM (UNIDADE: MXKM). AF_07/2019</t>
   </si>
   <si>
     <t xml:space="preserve">UND</t>
@@ -9183,9 +9180,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>180000</xdr:colOff>
+      <xdr:colOff>179640</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>120960</xdr:rowOff>
+      <xdr:rowOff>120600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9199,7 +9196,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1824480" y="1857240"/>
-          <a:ext cx="6320880" cy="4016880"/>
+          <a:ext cx="6320520" cy="4016520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9220,9 +9217,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>211680</xdr:colOff>
+      <xdr:colOff>211320</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>60480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9236,7 +9233,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1796040" y="5930280"/>
-          <a:ext cx="6381000" cy="4074840"/>
+          <a:ext cx="6380640" cy="4074480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9257,9 +9254,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>205920</xdr:colOff>
+      <xdr:colOff>205560</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>27720</xdr:rowOff>
+      <xdr:rowOff>27360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9273,7 +9270,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1786320" y="10119960"/>
-          <a:ext cx="6384960" cy="4042800"/>
+          <a:ext cx="6384600" cy="4042440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9299,9 +9296,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>913320</xdr:colOff>
+      <xdr:colOff>912960</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:rowOff>143640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9315,7 +9312,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7629840" y="5600880"/>
-          <a:ext cx="4384080" cy="722880"/>
+          <a:ext cx="4383720" cy="722520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9336,9 +9333,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>199080</xdr:colOff>
+      <xdr:colOff>198720</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>160920</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9348,7 +9345,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1064160" y="0"/>
-          <a:ext cx="8315280" cy="970560"/>
+          <a:ext cx="8314920" cy="970200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9425,9 +9422,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2210400</xdr:colOff>
+      <xdr:colOff>2210040</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>122040</xdr:rowOff>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9441,7 +9438,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="171360" y="390600"/>
-          <a:ext cx="3103200" cy="1053360"/>
+          <a:ext cx="3102840" cy="1053000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9457,19 +9454,6 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="DADOS"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -9507,6 +9491,19 @@
       <sheetData sheetId="13"/>
       <sheetData sheetId="14"/>
       <sheetData sheetId="15"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="DADOS"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -9559,6 +9556,61 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="PLANILHA MEDIÇÃO COMPLETA"/>
+      <sheetName val="CRONOGRAMA"/>
+      <sheetName val="Relatório"/>
+      <sheetName val="Parecer Gerado"/>
+      <sheetName val="PARECERES"/>
+      <sheetName val="HISTÓRICO DE PARECERES"/>
+      <sheetName val=" "/>
+      <sheetName val="FOLHA FECHAMENTO"/>
+      <sheetName val="PLANILHA_MEDIÇÃO_COMPLETA"/>
+      <sheetName val="Parecer_Gerado"/>
+      <sheetName val="HISTÓRICO_DE_PARECERES"/>
+      <sheetName val="_"/>
+      <sheetName val="PLANILHA_MEDIÇÃO_COMPLETA1"/>
+      <sheetName val="Parecer_Gerado1"/>
+      <sheetName val="HISTÓRICO_DE_PARECERES1"/>
+      <sheetName val="_1"/>
+      <sheetName val="Auxiliar FxF"/>
+      <sheetName val="cotações"/>
+      <sheetName val="insumos"/>
+      <sheetName val="serviços"/>
+      <sheetName val="Teor"/>
+      <sheetName val="compos1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
       <sheetName val="FOLHA FECHAMENTO"/>
     </sheetNames>
     <sheetDataSet>
@@ -9568,7 +9620,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -9583,7 +9635,32 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Orçamento"/>
+      <sheetName val="PATO"/>
+      <sheetName val="Cron_24 meses"/>
+      <sheetName val="Quad_Transp_"/>
+      <sheetName val="Aquisição Mat.Betum"/>
+      <sheetName val="Transp.Mat.Betum"/>
+      <sheetName val="CROQUI"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -9657,86 +9734,6 @@
       <sheetData sheetId="31"/>
       <sheetData sheetId="32"/>
       <sheetData sheetId="33"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="PLANILHA MEDIÇÃO COMPLETA"/>
-      <sheetName val="CRONOGRAMA"/>
-      <sheetName val="Relatório"/>
-      <sheetName val="Parecer Gerado"/>
-      <sheetName val="PARECERES"/>
-      <sheetName val="HISTÓRICO DE PARECERES"/>
-      <sheetName val=" "/>
-      <sheetName val="FOLHA FECHAMENTO"/>
-      <sheetName val="PLANILHA_MEDIÇÃO_COMPLETA"/>
-      <sheetName val="Parecer_Gerado"/>
-      <sheetName val="HISTÓRICO_DE_PARECERES"/>
-      <sheetName val="_"/>
-      <sheetName val="PLANILHA_MEDIÇÃO_COMPLETA1"/>
-      <sheetName val="Parecer_Gerado1"/>
-      <sheetName val="HISTÓRICO_DE_PARECERES1"/>
-      <sheetName val="_1"/>
-      <sheetName val="Auxiliar FxF"/>
-      <sheetName val="cotações"/>
-      <sheetName val="insumos"/>
-      <sheetName val="serviços"/>
-      <sheetName val="Teor"/>
-      <sheetName val="compos1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Orçamento"/>
-      <sheetName val="PATO"/>
-      <sheetName val="Cron_24 meses"/>
-      <sheetName val="Quad_Transp_"/>
-      <sheetName val="Aquisição Mat.Betum"/>
-      <sheetName val="Transp.Mat.Betum"/>
-      <sheetName val="CROQUI"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -15809,7 +15806,7 @@
         <v>74</v>
       </c>
       <c r="D116" s="137" t="s">
-        <v>209</v>
+        <v>144</v>
       </c>
       <c r="E116" s="137" t="s">
         <v>145</v>
@@ -16205,13 +16202,13 @@
         <v>29</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D5" s="46" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="49" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F5" s="49"/>
       <c r="G5" s="49"/>
@@ -16298,7 +16295,7 @@
       <c r="B10" s="60"/>
       <c r="C10" s="61"/>
       <c r="D10" s="61" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E10" s="178"/>
       <c r="F10" s="178"/>
@@ -16341,7 +16338,7 @@
       <c r="C12" s="61"/>
       <c r="D12" s="61"/>
       <c r="E12" s="178" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F12" s="178"/>
       <c r="G12" s="178"/>
@@ -16378,10 +16375,10 @@
       <c r="B14" s="60"/>
       <c r="C14" s="61"/>
       <c r="D14" s="61" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E14" s="178" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F14" s="178"/>
       <c r="G14" s="178"/>
@@ -16430,7 +16427,7 @@
       <c r="C16" s="61"/>
       <c r="D16" s="61"/>
       <c r="E16" s="178" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F16" s="178"/>
       <c r="G16" s="178"/>
@@ -16465,10 +16462,10 @@
       <c r="B18" s="60"/>
       <c r="C18" s="61"/>
       <c r="D18" s="61" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E18" s="178" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F18" s="178"/>
       <c r="G18" s="178"/>
@@ -16544,10 +16541,10 @@
       <c r="B22" s="60"/>
       <c r="C22" s="61"/>
       <c r="D22" s="61" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E22" s="178" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F22" s="178"/>
       <c r="G22" s="178"/>
@@ -16623,10 +16620,10 @@
       <c r="B26" s="60"/>
       <c r="C26" s="61"/>
       <c r="D26" s="61" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E26" s="178" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F26" s="178"/>
       <c r="G26" s="178"/>
@@ -16685,10 +16682,10 @@
       <c r="B29" s="60"/>
       <c r="C29" s="61"/>
       <c r="D29" s="61" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E29" s="178" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F29" s="178"/>
       <c r="G29" s="178"/>
@@ -16746,10 +16743,10 @@
       <c r="B32" s="60"/>
       <c r="C32" s="61"/>
       <c r="D32" s="61" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E32" s="178" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F32" s="178"/>
       <c r="G32" s="178"/>
@@ -16796,7 +16793,7 @@
         <v>2</v>
       </c>
       <c r="G34" s="184" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H34" s="180"/>
       <c r="K34" s="65"/>
@@ -16809,10 +16806,10 @@
       <c r="B35" s="74"/>
       <c r="C35" s="75"/>
       <c r="D35" s="61" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E35" s="178" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F35" s="178"/>
       <c r="G35" s="178"/>
@@ -16877,7 +16874,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="191" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H38" s="187"/>
       <c r="K38" s="192"/>
@@ -16897,7 +16894,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="191" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H39" s="179"/>
       <c r="K39" s="192"/>
@@ -16917,7 +16914,7 @@
         <v>2</v>
       </c>
       <c r="G40" s="191" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H40" s="179"/>
       <c r="K40" s="192"/>
@@ -16937,7 +16934,7 @@
         <v>3.17</v>
       </c>
       <c r="G41" s="191" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H41" s="179"/>
       <c r="K41" s="192"/>
@@ -16950,10 +16947,10 @@
       <c r="B42" s="189"/>
       <c r="C42" s="190"/>
       <c r="D42" s="61" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E42" s="178" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F42" s="191"/>
       <c r="G42" s="193"/>
@@ -17236,7 +17233,7 @@
       <c r="A1" s="198"/>
       <c r="B1" s="199"/>
       <c r="C1" s="200" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D1" s="200" t="s">
         <v>108</v>
@@ -17256,13 +17253,13 @@
       <c r="A2" s="201"/>
       <c r="B2" s="202"/>
       <c r="C2" s="203" t="s">
+        <v>223</v>
+      </c>
+      <c r="D2" s="203" t="s">
         <v>224</v>
       </c>
-      <c r="D2" s="203" t="s">
+      <c r="E2" s="203" t="s">
         <v>225</v>
-      </c>
-      <c r="E2" s="203" t="s">
-        <v>226</v>
       </c>
       <c r="F2" s="203"/>
       <c r="G2" s="203"/>
@@ -17274,7 +17271,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="204" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B3" s="204"/>
       <c r="C3" s="204"/>
@@ -17306,7 +17303,7 @@
         <v>33</v>
       </c>
       <c r="G4" s="205" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H4" s="205" t="s">
         <v>40</v>
@@ -17315,7 +17312,7 @@
         <v>37</v>
       </c>
       <c r="J4" s="205" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17659,7 +17656,7 @@
       <c r="D17" s="222"/>
       <c r="E17" s="223"/>
       <c r="F17" s="224" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G17" s="224"/>
       <c r="H17" s="225" t="n">
@@ -17702,7 +17699,7 @@
     </row>
     <row r="20" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="232" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B20" s="232"/>
       <c r="C20" s="232"/>
@@ -17771,21 +17768,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F1" s="234" t="s">
+        <v>231</v>
+      </c>
+      <c r="G1" s="235" t="s">
         <v>232</v>
       </c>
-      <c r="G1" s="235" t="s">
+      <c r="H1" s="236" t="s">
         <v>233</v>
       </c>
-      <c r="H1" s="236" t="s">
+      <c r="I1" s="237" t="s">
         <v>234</v>
-      </c>
-      <c r="I1" s="237" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="238" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E2" s="238"/>
       <c r="F2" s="239" t="n">
@@ -17801,24 +17798,24 @@
     </row>
     <row r="3" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="242" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E3" s="242"/>
       <c r="F3" s="243" t="s">
+        <v>237</v>
+      </c>
+      <c r="G3" s="244" t="s">
         <v>238</v>
       </c>
-      <c r="G3" s="244" t="s">
+      <c r="H3" s="245" t="s">
         <v>239</v>
-      </c>
-      <c r="H3" s="245" t="s">
-        <v>240</v>
       </c>
       <c r="I3" s="237"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="246"/>
       <c r="D4" s="242" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E4" s="242"/>
       <c r="F4" s="243"/>
@@ -17829,17 +17826,17 @@
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="246"/>
       <c r="D5" s="248" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E5" s="248"/>
       <c r="F5" s="249" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G5" s="250" t="s">
+        <v>242</v>
+      </c>
+      <c r="H5" s="251" t="s">
         <v>243</v>
-      </c>
-      <c r="H5" s="251" t="s">
-        <v>244</v>
       </c>
       <c r="I5" s="237"/>
     </row>
@@ -17848,35 +17845,35 @@
         <v>14</v>
       </c>
       <c r="B6" s="253" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C6" s="253"/>
       <c r="D6" s="253"/>
       <c r="E6" s="254" t="s">
+        <v>245</v>
+      </c>
+      <c r="F6" s="253" t="s">
         <v>246</v>
       </c>
-      <c r="F6" s="253" t="s">
-        <v>247</v>
-      </c>
       <c r="G6" s="253" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H6" s="253" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I6" s="255"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="256" t="s">
+        <v>247</v>
+      </c>
+      <c r="B7" s="257" t="s">
         <v>248</v>
-      </c>
-      <c r="B7" s="257" t="s">
-        <v>249</v>
       </c>
       <c r="C7" s="257"/>
       <c r="D7" s="257"/>
       <c r="E7" s="257" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F7" s="258" t="n">
         <v>12.91</v>
@@ -17978,7 +17975,7 @@
     </row>
     <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="264" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B3" s="264"/>
       <c r="C3" s="264"/>
@@ -18030,7 +18027,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="271" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B6" s="266" t="str">
         <f aca="false">Resumo!B3</f>
@@ -18071,10 +18068,10 @@
         <v>31</v>
       </c>
       <c r="C8" s="276" t="s">
+        <v>251</v>
+      </c>
+      <c r="D8" s="276" t="s">
         <v>252</v>
-      </c>
-      <c r="D8" s="276" t="s">
-        <v>253</v>
       </c>
       <c r="E8" s="276"/>
       <c r="F8" s="276"/>
@@ -18539,7 +18536,7 @@
     </row>
     <row r="28" s="282" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="276" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B28" s="276"/>
       <c r="C28" s="285" t="n">
@@ -18591,7 +18588,7 @@
     </row>
     <row r="29" s="282" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="276" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B29" s="276"/>
       <c r="C29" s="287" t="n">
@@ -18642,7 +18639,7 @@
     </row>
     <row r="30" s="282" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="276" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B30" s="276"/>
       <c r="C30" s="285" t="n">
@@ -18694,7 +18691,7 @@
     </row>
     <row r="31" s="282" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="276" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B31" s="276"/>
       <c r="C31" s="289" t="n">
@@ -18904,7 +18901,7 @@
     <row r="7" s="295" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="298"/>
       <c r="C7" s="299" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D7" s="300" t="str">
         <f aca="false">IF([9]DADOS!$D$12&lt;&gt;"",[9]DADOS!$D$12," ")</f>
@@ -18919,14 +18916,14 @@
     <row r="8" s="295" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="298"/>
       <c r="C8" s="299" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D8" s="302" t="str">
         <f aca="false">IF('[9]FOLHA FECHAMENTO'!F31&lt;&gt;"",'[9]FOLHA FECHAMENTO'!F31," ")</f>
         <v> </v>
       </c>
       <c r="E8" s="300" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F8" s="301"/>
       <c r="G8" s="301"/>
@@ -18936,12 +18933,12 @@
     <row r="9" s="295" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="303"/>
       <c r="C9" s="304" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D9" s="305"/>
       <c r="E9" s="306"/>
       <c r="H9" s="307" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I9" s="307"/>
     </row>
@@ -18950,7 +18947,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="308" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B11" s="308"/>
       <c r="C11" s="308"/>
@@ -18969,22 +18966,22 @@
         <v>14</v>
       </c>
       <c r="B12" s="310" t="s">
+        <v>263</v>
+      </c>
+      <c r="C12" s="310" t="s">
         <v>264</v>
       </c>
-      <c r="C12" s="310" t="s">
+      <c r="D12" s="310" t="s">
         <v>265</v>
       </c>
-      <c r="D12" s="310" t="s">
+      <c r="E12" s="311" t="s">
         <v>266</v>
       </c>
-      <c r="E12" s="311" t="s">
+      <c r="F12" s="311" t="s">
         <v>267</v>
       </c>
-      <c r="F12" s="311" t="s">
+      <c r="G12" s="310" t="s">
         <v>268</v>
-      </c>
-      <c r="G12" s="310" t="s">
-        <v>269</v>
       </c>
       <c r="H12" s="310"/>
       <c r="I12" s="310"/>
@@ -18997,13 +18994,13 @@
       <c r="E13" s="311"/>
       <c r="F13" s="311"/>
       <c r="G13" s="310" t="s">
+        <v>269</v>
+      </c>
+      <c r="H13" s="310" t="s">
         <v>270</v>
       </c>
-      <c r="H13" s="310" t="s">
+      <c r="I13" s="310" t="s">
         <v>271</v>
-      </c>
-      <c r="I13" s="310" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19011,7 +19008,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="314" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C14" s="315" t="n">
         <f aca="false">D14*$I$11</f>
@@ -19035,10 +19032,10 @@
         <v>0.055</v>
       </c>
       <c r="J14" s="293" t="s">
+        <v>273</v>
+      </c>
+      <c r="K14" s="293" t="s">
         <v>274</v>
-      </c>
-      <c r="K14" s="293" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19046,7 +19043,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="314" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C15" s="315" t="n">
         <f aca="false">D15*$I$11</f>
@@ -19070,10 +19067,10 @@
         <v>0.01</v>
       </c>
       <c r="J15" s="293" t="s">
+        <v>276</v>
+      </c>
+      <c r="K15" s="293" t="s">
         <v>277</v>
-      </c>
-      <c r="K15" s="293" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19081,7 +19078,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="314" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C16" s="315" t="n">
         <f aca="false">D16*$I$11</f>
@@ -19105,10 +19102,10 @@
         <v>0.0127</v>
       </c>
       <c r="J16" s="293" t="s">
+        <v>279</v>
+      </c>
+      <c r="K16" s="293" t="s">
         <v>280</v>
-      </c>
-      <c r="K16" s="293" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19116,7 +19113,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="314" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C17" s="315" t="n">
         <f aca="false">D17*($I$11+C14+C15+C16)</f>
@@ -19140,10 +19137,10 @@
         <v>0.0139</v>
       </c>
       <c r="J17" s="293" t="s">
+        <v>282</v>
+      </c>
+      <c r="K17" s="293" t="s">
         <v>283</v>
-      </c>
-      <c r="K17" s="293" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19151,7 +19148,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="314" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C18" s="315" t="n">
         <f aca="false">D18*($I$11+C14+C15+C16+C17)</f>
@@ -19178,7 +19175,7 @@
         <v>126</v>
       </c>
       <c r="K18" s="293" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19186,7 +19183,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="319" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C19" s="320" t="n">
         <f aca="false">D19*$I$11*(1+D26)</f>
@@ -19202,18 +19199,18 @@
       <c r="H19" s="323"/>
       <c r="I19" s="324"/>
       <c r="J19" s="293" t="s">
+        <v>287</v>
+      </c>
+      <c r="K19" s="293" t="s">
         <v>288</v>
-      </c>
-      <c r="K19" s="293" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="325" t="s">
+        <v>289</v>
+      </c>
+      <c r="B20" s="326" t="s">
         <v>290</v>
-      </c>
-      <c r="B20" s="326" t="s">
-        <v>291</v>
       </c>
       <c r="C20" s="326"/>
       <c r="D20" s="318" t="n">
@@ -19227,10 +19224,10 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="325" t="s">
+        <v>291</v>
+      </c>
+      <c r="B21" s="326" t="s">
         <v>292</v>
-      </c>
-      <c r="B21" s="326" t="s">
-        <v>293</v>
       </c>
       <c r="C21" s="326"/>
       <c r="D21" s="318" t="n">
@@ -19244,10 +19241,10 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="325" t="s">
+        <v>293</v>
+      </c>
+      <c r="B22" s="326" t="s">
         <v>294</v>
-      </c>
-      <c r="B22" s="326" t="s">
-        <v>295</v>
       </c>
       <c r="C22" s="326"/>
       <c r="D22" s="318" t="n">
@@ -19261,10 +19258,10 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="325" t="s">
+        <v>295</v>
+      </c>
+      <c r="B23" s="326" t="s">
         <v>296</v>
-      </c>
-      <c r="B23" s="326" t="s">
-        <v>297</v>
       </c>
       <c r="C23" s="326"/>
       <c r="D23" s="328" t="n">
@@ -19279,7 +19276,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="313" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B24" s="313"/>
       <c r="C24" s="329" t="n">
@@ -19289,7 +19286,7 @@
       <c r="D24" s="313"/>
       <c r="E24" s="313"/>
       <c r="F24" s="313" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G24" s="313"/>
       <c r="H24" s="313"/>
@@ -19297,7 +19294,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="313" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B25" s="313"/>
       <c r="C25" s="329" t="n">
@@ -19307,7 +19304,7 @@
       <c r="D25" s="313"/>
       <c r="E25" s="313"/>
       <c r="F25" s="330" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G25" s="317" t="n">
         <v>0.2034</v>
@@ -19322,7 +19319,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="313" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B26" s="313"/>
       <c r="C26" s="313"/>
@@ -19335,7 +19332,7 @@
         <v>OK</v>
       </c>
       <c r="F26" s="330" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G26" s="317" t="n">
         <f aca="false">((G25+1)*(1-E29))/((1-E29)-D23)-1</f>
@@ -19368,7 +19365,7 @@
       <c r="D28" s="295"/>
       <c r="E28" s="296"/>
       <c r="F28" s="333" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G28" s="334"/>
       <c r="H28" s="334"/>
@@ -19409,7 +19406,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="295" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B32" s="295"/>
       <c r="C32" s="295"/>
@@ -19422,7 +19419,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="295" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B33" s="295"/>
       <c r="C33" s="295"/>
@@ -19435,7 +19432,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="295" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B34" s="295"/>
       <c r="C34" s="295"/>
@@ -19448,7 +19445,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="295" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B35" s="295"/>
       <c r="C35" s="295"/>
@@ -19461,7 +19458,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="295" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B36" s="295"/>
       <c r="C36" s="295"/>
@@ -19474,7 +19471,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="295" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B37" s="295"/>
       <c r="C37" s="295"/>
@@ -19487,7 +19484,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="295" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B38" s="295"/>
       <c r="C38" s="295"/>
@@ -19500,7 +19497,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="295" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B39" s="295"/>
       <c r="C39" s="295"/>
@@ -19532,7 +19529,7 @@
       <c r="D41" s="295"/>
       <c r="E41" s="296"/>
       <c r="F41" s="342" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G41" s="342"/>
       <c r="H41" s="342"/>
@@ -19545,7 +19542,7 @@
       <c r="D42" s="295"/>
       <c r="E42" s="296"/>
       <c r="F42" s="342" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G42" s="342"/>
       <c r="H42" s="342"/>

</xml_diff>

<commit_message>
feat: Update structure validation scripts and output files for improved functionality and filtering by bank
</commit_message>
<xml_diff>
--- a/data/ORÇAMENTO - ACIONAMENTO 01 - REV 05 final.xlsx
+++ b/data/ORÇAMENTO - ACIONAMENTO 01 - REV 05 final.xlsx
@@ -9180,9 +9180,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>179640</xdr:colOff>
+      <xdr:colOff>179280</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>120600</xdr:rowOff>
+      <xdr:rowOff>120240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9196,7 +9196,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1824480" y="1857240"/>
-          <a:ext cx="6320520" cy="4016520"/>
+          <a:ext cx="6320160" cy="4016160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9217,9 +9217,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>211320</xdr:colOff>
+      <xdr:colOff>210960</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9233,7 +9233,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1796040" y="5930280"/>
-          <a:ext cx="6380640" cy="4074480"/>
+          <a:ext cx="6380280" cy="4074120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9254,9 +9254,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>205560</xdr:colOff>
+      <xdr:colOff>205200</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>27360</xdr:rowOff>
+      <xdr:rowOff>27000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9270,7 +9270,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1786320" y="10119960"/>
-          <a:ext cx="6384600" cy="4042440"/>
+          <a:ext cx="6384240" cy="4042080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9296,9 +9296,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>912960</xdr:colOff>
+      <xdr:colOff>912600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:rowOff>143280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9312,7 +9312,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7629840" y="5600880"/>
-          <a:ext cx="4383720" cy="722520"/>
+          <a:ext cx="4383360" cy="722160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9333,9 +9333,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>198720</xdr:colOff>
+      <xdr:colOff>198360</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9345,7 +9345,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1064160" y="0"/>
-          <a:ext cx="8314920" cy="970200"/>
+          <a:ext cx="8314560" cy="969840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9422,9 +9422,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2210040</xdr:colOff>
+      <xdr:colOff>2209680</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>121680</xdr:rowOff>
+      <xdr:rowOff>121320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9438,7 +9438,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="171360" y="390600"/>
-          <a:ext cx="3102840" cy="1053000"/>
+          <a:ext cx="3102480" cy="1052640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9454,6 +9454,19 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="DADOS"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -9491,19 +9504,6 @@
       <sheetData sheetId="13"/>
       <sheetData sheetId="14"/>
       <sheetData sheetId="15"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="DADOS"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -9553,6 +9553,31 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Orçamento"/>
+      <sheetName val="PATO"/>
+      <sheetName val="Cron_24 meses"/>
+      <sheetName val="Quad_Transp_"/>
+      <sheetName val="Aquisição Mat.Betum"/>
+      <sheetName val="Transp.Mat.Betum"/>
+      <sheetName val="CROQUI"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -9607,7 +9632,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -9620,47 +9645,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Serviços"/>
-      <sheetName val="Dados_da_Obra"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Orçamento"/>
-      <sheetName val="PATO"/>
-      <sheetName val="Cron_24 meses"/>
-      <sheetName val="Quad_Transp_"/>
-      <sheetName val="Aquisição Mat.Betum"/>
-      <sheetName val="Transp.Mat.Betum"/>
-      <sheetName val="CROQUI"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -9734,6 +9719,21 @@
       <sheetData sheetId="31"/>
       <sheetData sheetId="32"/>
       <sheetData sheetId="33"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Serviços"/>
+      <sheetName val="Dados_da_Obra"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -12176,8 +12176,8 @@
   </sheetPr>
   <dimension ref="A1:L125"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat: Implement JSON output for price comparisons and structure validation
- Added JSON output files for price comparisons with SUDECAP and SINAPI.
- Removed Excel export functionality for price comparisons.
- Introduced new commands for running price comparisons and validating structures.
- Updated CLI to support new JSON output format and added helper functions for JSON export.
- Created bash commands for manual and automatic execution of price comparison and structure validation.
- Added new JSON structure for storing divergences in price and structure comparisons.
</commit_message>
<xml_diff>
--- a/data/ORÇAMENTO - ACIONAMENTO 01 - REV 05 final.xlsx
+++ b/data/ORÇAMENTO - ACIONAMENTO 01 - REV 05 final.xlsx
@@ -5547,7 +5547,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="316">
   <si>
     <t xml:space="preserve">RESUMO</t>
   </si>
@@ -5916,7 +5916,7 @@
     <t xml:space="preserve">Mão de Obra</t>
   </si>
   <si>
-    <t xml:space="preserve"> 55.15.07 </t>
+    <t xml:space="preserve"> 55.15.17 </t>
   </si>
   <si>
     <t xml:space="preserve">TÉCNICO INTERMEDIÁRIO</t>
@@ -5925,7 +5925,7 @@
     <t xml:space="preserve"> 68.01.03 </t>
   </si>
   <si>
-    <t xml:space="preserve">ETANOL</t>
+    <t xml:space="preserve">ETANOL1</t>
   </si>
   <si>
     <t xml:space="preserve">Material</t>
@@ -5982,202 +5982,208 @@
     <t xml:space="preserve">Composição Auxiliar</t>
   </si>
   <si>
+    <t xml:space="preserve"> 103251 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSPORTE HORIZONTAL MANUAL, DE TUBO DE AÇO CARBONO LEVE OU MÉDIO, PRETO OU GALVANIZADO, COM DIÂMETRO MAIOR QUE 32 MM E MENOR OU IGUAL A 65 MM (UNIDADE: MXKM). AF_07/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transporte de Materiais dentro do Canteiro de Obras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MXKM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 88278 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONTADOR DE ESTRUTURA METÁLICA COM ENCARGOS COMPLEMENTARES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Livro SINAPI: Cálculos e Parâmetros</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 88316 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERVENTE COM ENCARGOS COMPLEMENTARES1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSTALACOES ELETRICAS - LEITOS E CABOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 099250 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELETRICISTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 099806 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AJUDANTE DE ELETRICISTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B.01.000.010116 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajudante eletricista</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B.01.000.010115 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eletricista</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B.07.000.049501 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fita isolante de 20 m, ref. 3M Scoth 33MR ou equivalente - uso especial</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P.15.000.090205 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luminária LED quadrada, sobrepor, de 15 a 24W fluxo lum. 1363 a 1800 lm, 220V, temper. de cor 4000 K, difusor prismático transparente; ref. 400-24/1 LED da ARM, EF75-S2000840, difusor leitoso Lumicenter, PL 289/LED18W TL Prolumi ou equivalente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSTALACOES ELETRICAS - LUMINARIAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 003420 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FITA ISOLANTE HIGHLAND ADESIVA 19m x 20mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 203066 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRIVER DE REPOSICAO PARA PLAFON DE LED EMBUTIR E SOBREPOR 36W</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 88264 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 95332 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURSO DE CAPACITAÇÃO PARA ELETRICISTA (ENCARGOS COMPLEMENTARES) - HORISTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00002436 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELETRICISTA (HORISTA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00037370 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIMENTACAO - HORISTA (COLETADO CAIXA - ENCARGOS COMPLEMENTARES)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00037371 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSPORTE - HORISTA (COLETADO CAIXA - ENCARGOS COMPLEMENTARES)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00037372 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXAMES - HORISTA (COLETADO CAIXA - ENCARGOS COMPLEMENTARES)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00037373 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEGURO - HORISTA (COLETADO CAIXA - ENCARGOS COMPLEMENTARES)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00043460 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERRAMENTAS - FAMILIA ELETRICISTA - HORISTA (ENCARGOS COMPLEMENTARES - COLETADO CAIXA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00043484 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPI - FAMILIA ELETRICISTA - HORISTA (ENCARGOS COMPLEMENTARES - COLETADO CAIXA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5.1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 020408 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PREPARACAO DO TERRENO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 099900 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERVENTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Composições Auxiliares</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 95344 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURSO DE CAPACITAÇÃO PARA MONTADOR DE ESTRUTURA METÁLICA (ENCARGOS COMPLEMENTARES) - HORISTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00044497 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONTADOR DE ESTRUTURAS METALICAS HORISTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 95378 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURSO DE CAPACITAÇÃO PARA SERVENTE (ENCARGOS COMPLEMENTARES) - HORISTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00006111 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERVENTE DE OBRAS (HORISTA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00043464 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERRAMENTAS - FAMILIA OPERADOR ESCAVADEIRA - HORISTA (ENCARGOS COMPLEMENTARES - COLETADO CAIXA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00043488 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPI - FAMILIA OPERADOR ESCAVADEIRA - HORISTA (ENCARGOS COMPLEMENTARES - COLETADO CAIXA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERVENTE COM ENCARGOS COMPLEMENTARES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00043467 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERRAMENTAS - FAMILIA SERVENTE - HORISTA (ENCARGOS COMPLEMENTARES - COLETADO CAIXA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00043491 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPI - FAMILIA SERVENTE - HORISTA (ENCARGOS COMPLEMENTARES - COLETADO CAIXA)</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 100251 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSPORTE HORIZONTAL MANUAL, DE TUBO DE AÇO CARBONO LEVE OU MÉDIO, PRETO OU GALVANIZADO, COM DIÂMETRO MAIOR QUE 32 MM E MENOR OU IGUAL A 65 MM (UNIDADE: MXKM). AF_07/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transporte de Materiais dentro do Canteiro de Obras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MXKM</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 88278 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MONTADOR DE ESTRUTURA METÁLICA COM ENCARGOS COMPLEMENTARES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Livro SINAPI: Cálculos e Parâmetros</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 88316 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SERVENTE COM ENCARGOS COMPLEMENTARES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INSTALACOES ELETRICAS - LEITOS E CABOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 099250 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELETRICISTA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 099806 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AJUDANTE DE ELETRICISTA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> B.01.000.010116 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajudante eletricista</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> B.01.000.010115 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eletricista</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> B.07.000.049501 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fita isolante de 20 m, ref. 3M Scoth 33MR ou equivalente - uso especial</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> P.15.000.090205 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luminária LED quadrada, sobrepor, de 15 a 24W fluxo lum. 1363 a 1800 lm, 220V, temper. de cor 4000 K, difusor prismático transparente; ref. 400-24/1 LED da ARM, EF75-S2000840, difusor leitoso Lumicenter, PL 289/LED18W TL Prolumi ou equivalente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INSTALACOES ELETRICAS - LUMINARIAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 003420 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FITA ISOLANTE HIGHLAND ADESIVA 19m x 20mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 203066 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DRIVER DE REPOSICAO PARA PLAFON DE LED EMBUTIR E SOBREPOR 36W</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 88264 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 95332 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CURSO DE CAPACITAÇÃO PARA ELETRICISTA (ENCARGOS COMPLEMENTARES) - HORISTA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 00002436 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELETRICISTA (HORISTA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 00037370 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALIMENTACAO - HORISTA (COLETADO CAIXA - ENCARGOS COMPLEMENTARES)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 00037371 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSPORTE - HORISTA (COLETADO CAIXA - ENCARGOS COMPLEMENTARES)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 00037372 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXAMES - HORISTA (COLETADO CAIXA - ENCARGOS COMPLEMENTARES)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 00037373 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEGURO - HORISTA (COLETADO CAIXA - ENCARGOS COMPLEMENTARES)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 00043460 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FERRAMENTAS - FAMILIA ELETRICISTA - HORISTA (ENCARGOS COMPLEMENTARES - COLETADO CAIXA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 00043484 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EPI - FAMILIA ELETRICISTA - HORISTA (ENCARGOS COMPLEMENTARES - COLETADO CAIXA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5.1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 020408 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PREPARACAO DO TERRENO</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 099900 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SERVENTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Composições Auxiliares</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 95344 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CURSO DE CAPACITAÇÃO PARA MONTADOR DE ESTRUTURA METÁLICA (ENCARGOS COMPLEMENTARES) - HORISTA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 00044497 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MONTADOR DE ESTRUTURAS METALICAS HORISTA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 95378 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CURSO DE CAPACITAÇÃO PARA SERVENTE (ENCARGOS COMPLEMENTARES) - HORISTA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 00006111 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SERVENTE DE OBRAS (HORISTA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 00043464 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FERRAMENTAS - FAMILIA OPERADOR ESCAVADEIRA - HORISTA (ENCARGOS COMPLEMENTARES - COLETADO CAIXA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 00043488 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EPI - FAMILIA OPERADOR ESCAVADEIRA - HORISTA (ENCARGOS COMPLEMENTARES - COLETADO CAIXA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 00043467 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FERRAMENTAS - FAMILIA SERVENTE - HORISTA (ENCARGOS COMPLEMENTARES - COLETADO CAIXA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 00043491 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EPI - FAMILIA SERVENTE - HORISTA (ENCARGOS COMPLEMENTARES - COLETADO CAIXA)</t>
   </si>
   <si>
     <t xml:space="preserve">UND</t>
@@ -12176,8 +12182,8 @@
   </sheetPr>
   <dimension ref="A1:L125"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12954,7 +12960,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="140" t="n">
-        <v>362.45</v>
+        <v>362.44</v>
       </c>
       <c r="J6" s="141" t="n">
         <v>362.45</v>
@@ -13311,7 +13317,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="140" t="n">
-        <v>30.78</v>
+        <v>30.79</v>
       </c>
       <c r="J19" s="141" t="n">
         <v>30.78</v>
@@ -15452,7 +15458,7 @@
         <v>74</v>
       </c>
       <c r="D103" s="137" t="s">
-        <v>151</v>
+        <v>205</v>
       </c>
       <c r="E103" s="137" t="s">
         <v>149</v>
@@ -15656,13 +15662,13 @@
         <v>113</v>
       </c>
       <c r="B110" s="158" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C110" s="145" t="s">
         <v>74</v>
       </c>
       <c r="D110" s="145" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E110" s="145" t="s">
         <v>125</v>
@@ -15686,13 +15692,13 @@
         <v>113</v>
       </c>
       <c r="B111" s="158" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C111" s="145" t="s">
         <v>74</v>
       </c>
       <c r="D111" s="145" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E111" s="145" t="s">
         <v>125</v>
@@ -15800,7 +15806,7 @@
         <v>112</v>
       </c>
       <c r="B116" s="136" t="s">
-        <v>143</v>
+        <v>210</v>
       </c>
       <c r="C116" s="137" t="s">
         <v>74</v>
@@ -15836,7 +15842,7 @@
         <v>74</v>
       </c>
       <c r="D117" s="145" t="s">
-        <v>151</v>
+        <v>205</v>
       </c>
       <c r="E117" s="145" t="s">
         <v>149</v>
@@ -16202,13 +16208,13 @@
         <v>29</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D5" s="46" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="49" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F5" s="49"/>
       <c r="G5" s="49"/>
@@ -16295,7 +16301,7 @@
       <c r="B10" s="60"/>
       <c r="C10" s="61"/>
       <c r="D10" s="61" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E10" s="178"/>
       <c r="F10" s="178"/>
@@ -16338,7 +16344,7 @@
       <c r="C12" s="61"/>
       <c r="D12" s="61"/>
       <c r="E12" s="178" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F12" s="178"/>
       <c r="G12" s="178"/>
@@ -16375,10 +16381,10 @@
       <c r="B14" s="60"/>
       <c r="C14" s="61"/>
       <c r="D14" s="61" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E14" s="178" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F14" s="178"/>
       <c r="G14" s="178"/>
@@ -16427,7 +16433,7 @@
       <c r="C16" s="61"/>
       <c r="D16" s="61"/>
       <c r="E16" s="178" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F16" s="178"/>
       <c r="G16" s="178"/>
@@ -16462,10 +16468,10 @@
       <c r="B18" s="60"/>
       <c r="C18" s="61"/>
       <c r="D18" s="61" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E18" s="178" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F18" s="178"/>
       <c r="G18" s="178"/>
@@ -16541,10 +16547,10 @@
       <c r="B22" s="60"/>
       <c r="C22" s="61"/>
       <c r="D22" s="61" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E22" s="178" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F22" s="178"/>
       <c r="G22" s="178"/>
@@ -16620,10 +16626,10 @@
       <c r="B26" s="60"/>
       <c r="C26" s="61"/>
       <c r="D26" s="61" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E26" s="178" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F26" s="178"/>
       <c r="G26" s="178"/>
@@ -16682,10 +16688,10 @@
       <c r="B29" s="60"/>
       <c r="C29" s="61"/>
       <c r="D29" s="61" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E29" s="178" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F29" s="178"/>
       <c r="G29" s="178"/>
@@ -16743,10 +16749,10 @@
       <c r="B32" s="60"/>
       <c r="C32" s="61"/>
       <c r="D32" s="61" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E32" s="178" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F32" s="178"/>
       <c r="G32" s="178"/>
@@ -16793,7 +16799,7 @@
         <v>2</v>
       </c>
       <c r="G34" s="184" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H34" s="180"/>
       <c r="K34" s="65"/>
@@ -16806,10 +16812,10 @@
       <c r="B35" s="74"/>
       <c r="C35" s="75"/>
       <c r="D35" s="61" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E35" s="178" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F35" s="178"/>
       <c r="G35" s="178"/>
@@ -16874,7 +16880,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="191" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="H38" s="187"/>
       <c r="K38" s="192"/>
@@ -16894,7 +16900,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="191" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="H39" s="179"/>
       <c r="K39" s="192"/>
@@ -16914,7 +16920,7 @@
         <v>2</v>
       </c>
       <c r="G40" s="191" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="H40" s="179"/>
       <c r="K40" s="192"/>
@@ -16934,7 +16940,7 @@
         <v>3.17</v>
       </c>
       <c r="G41" s="191" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="H41" s="179"/>
       <c r="K41" s="192"/>
@@ -16947,10 +16953,10 @@
       <c r="B42" s="189"/>
       <c r="C42" s="190"/>
       <c r="D42" s="61" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E42" s="178" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F42" s="191"/>
       <c r="G42" s="193"/>
@@ -17233,7 +17239,7 @@
       <c r="A1" s="198"/>
       <c r="B1" s="199"/>
       <c r="C1" s="200" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D1" s="200" t="s">
         <v>108</v>
@@ -17253,13 +17259,13 @@
       <c r="A2" s="201"/>
       <c r="B2" s="202"/>
       <c r="C2" s="203" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D2" s="203" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E2" s="203" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F2" s="203"/>
       <c r="G2" s="203"/>
@@ -17271,7 +17277,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="204" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B3" s="204"/>
       <c r="C3" s="204"/>
@@ -17303,7 +17309,7 @@
         <v>33</v>
       </c>
       <c r="G4" s="205" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H4" s="205" t="s">
         <v>40</v>
@@ -17312,7 +17318,7 @@
         <v>37</v>
       </c>
       <c r="J4" s="205" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17656,7 +17662,7 @@
       <c r="D17" s="222"/>
       <c r="E17" s="223"/>
       <c r="F17" s="224" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="G17" s="224"/>
       <c r="H17" s="225" t="n">
@@ -17699,7 +17705,7 @@
     </row>
     <row r="20" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="232" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B20" s="232"/>
       <c r="C20" s="232"/>
@@ -17768,21 +17774,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F1" s="234" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="G1" s="235" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="H1" s="236" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="I1" s="237" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="238" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E2" s="238"/>
       <c r="F2" s="239" t="n">
@@ -17798,24 +17804,24 @@
     </row>
     <row r="3" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="242" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E3" s="242"/>
       <c r="F3" s="243" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="G3" s="244" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="H3" s="245" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="I3" s="237"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="246"/>
       <c r="D4" s="242" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E4" s="242"/>
       <c r="F4" s="243"/>
@@ -17826,17 +17832,17 @@
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="246"/>
       <c r="D5" s="248" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E5" s="248"/>
       <c r="F5" s="249" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="G5" s="250" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="H5" s="251" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="I5" s="237"/>
     </row>
@@ -17845,35 +17851,35 @@
         <v>14</v>
       </c>
       <c r="B6" s="253" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C6" s="253"/>
       <c r="D6" s="253"/>
       <c r="E6" s="254" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F6" s="253" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="G6" s="253" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="H6" s="253" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="I6" s="255"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="256" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B7" s="257" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C7" s="257"/>
       <c r="D7" s="257"/>
       <c r="E7" s="257" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="F7" s="258" t="n">
         <v>12.91</v>
@@ -17975,7 +17981,7 @@
     </row>
     <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="264" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B3" s="264"/>
       <c r="C3" s="264"/>
@@ -18027,7 +18033,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="271" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B6" s="266" t="str">
         <f aca="false">Resumo!B3</f>
@@ -18068,10 +18074,10 @@
         <v>31</v>
       </c>
       <c r="C8" s="276" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D8" s="276" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="E8" s="276"/>
       <c r="F8" s="276"/>
@@ -18536,7 +18542,7 @@
     </row>
     <row r="28" s="282" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="276" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B28" s="276"/>
       <c r="C28" s="285" t="n">
@@ -18588,7 +18594,7 @@
     </row>
     <row r="29" s="282" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="276" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B29" s="276"/>
       <c r="C29" s="287" t="n">
@@ -18639,7 +18645,7 @@
     </row>
     <row r="30" s="282" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="276" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B30" s="276"/>
       <c r="C30" s="285" t="n">
@@ -18691,7 +18697,7 @@
     </row>
     <row r="31" s="282" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="276" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B31" s="276"/>
       <c r="C31" s="289" t="n">
@@ -18901,7 +18907,7 @@
     <row r="7" s="295" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="298"/>
       <c r="C7" s="299" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D7" s="300" t="str">
         <f aca="false">IF([9]DADOS!$D$12&lt;&gt;"",[9]DADOS!$D$12," ")</f>
@@ -18916,14 +18922,14 @@
     <row r="8" s="295" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="298"/>
       <c r="C8" s="299" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D8" s="302" t="str">
         <f aca="false">IF('[9]FOLHA FECHAMENTO'!F31&lt;&gt;"",'[9]FOLHA FECHAMENTO'!F31," ")</f>
         <v> </v>
       </c>
       <c r="E8" s="300" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="F8" s="301"/>
       <c r="G8" s="301"/>
@@ -18933,12 +18939,12 @@
     <row r="9" s="295" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="303"/>
       <c r="C9" s="304" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D9" s="305"/>
       <c r="E9" s="306"/>
       <c r="H9" s="307" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="I9" s="307"/>
     </row>
@@ -18947,7 +18953,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="308" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B11" s="308"/>
       <c r="C11" s="308"/>
@@ -18966,22 +18972,22 @@
         <v>14</v>
       </c>
       <c r="B12" s="310" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C12" s="310" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D12" s="310" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="E12" s="311" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F12" s="311" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="G12" s="310" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="H12" s="310"/>
       <c r="I12" s="310"/>
@@ -18994,13 +19000,13 @@
       <c r="E13" s="311"/>
       <c r="F13" s="311"/>
       <c r="G13" s="310" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="H13" s="310" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="I13" s="310" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19008,7 +19014,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="314" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C14" s="315" t="n">
         <f aca="false">D14*$I$11</f>
@@ -19032,10 +19038,10 @@
         <v>0.055</v>
       </c>
       <c r="J14" s="293" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="K14" s="293" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19043,7 +19049,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="314" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C15" s="315" t="n">
         <f aca="false">D15*$I$11</f>
@@ -19067,10 +19073,10 @@
         <v>0.01</v>
       </c>
       <c r="J15" s="293" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="K15" s="293" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19078,7 +19084,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="314" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C16" s="315" t="n">
         <f aca="false">D16*$I$11</f>
@@ -19102,10 +19108,10 @@
         <v>0.0127</v>
       </c>
       <c r="J16" s="293" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="K16" s="293" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19113,7 +19119,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="314" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C17" s="315" t="n">
         <f aca="false">D17*($I$11+C14+C15+C16)</f>
@@ -19137,10 +19143,10 @@
         <v>0.0139</v>
       </c>
       <c r="J17" s="293" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="K17" s="293" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19148,7 +19154,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="314" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C18" s="315" t="n">
         <f aca="false">D18*($I$11+C14+C15+C16+C17)</f>
@@ -19175,7 +19181,7 @@
         <v>126</v>
       </c>
       <c r="K18" s="293" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19183,7 +19189,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="319" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C19" s="320" t="n">
         <f aca="false">D19*$I$11*(1+D26)</f>
@@ -19199,18 +19205,18 @@
       <c r="H19" s="323"/>
       <c r="I19" s="324"/>
       <c r="J19" s="293" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="K19" s="293" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="325" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B20" s="326" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C20" s="326"/>
       <c r="D20" s="318" t="n">
@@ -19224,10 +19230,10 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="325" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B21" s="326" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C21" s="326"/>
       <c r="D21" s="318" t="n">
@@ -19241,10 +19247,10 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="325" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B22" s="326" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C22" s="326"/>
       <c r="D22" s="318" t="n">
@@ -19258,10 +19264,10 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="325" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B23" s="326" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C23" s="326"/>
       <c r="D23" s="328" t="n">
@@ -19276,7 +19282,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="313" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B24" s="313"/>
       <c r="C24" s="329" t="n">
@@ -19286,7 +19292,7 @@
       <c r="D24" s="313"/>
       <c r="E24" s="313"/>
       <c r="F24" s="313" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="G24" s="313"/>
       <c r="H24" s="313"/>
@@ -19294,7 +19300,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="313" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B25" s="313"/>
       <c r="C25" s="329" t="n">
@@ -19304,7 +19310,7 @@
       <c r="D25" s="313"/>
       <c r="E25" s="313"/>
       <c r="F25" s="330" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="G25" s="317" t="n">
         <v>0.2034</v>
@@ -19319,7 +19325,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="313" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B26" s="313"/>
       <c r="C26" s="313"/>
@@ -19332,7 +19338,7 @@
         <v>OK</v>
       </c>
       <c r="F26" s="330" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="G26" s="317" t="n">
         <f aca="false">((G25+1)*(1-E29))/((1-E29)-D23)-1</f>
@@ -19365,7 +19371,7 @@
       <c r="D28" s="295"/>
       <c r="E28" s="296"/>
       <c r="F28" s="333" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="G28" s="334"/>
       <c r="H28" s="334"/>
@@ -19406,7 +19412,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="295" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B32" s="295"/>
       <c r="C32" s="295"/>
@@ -19419,7 +19425,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="295" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B33" s="295"/>
       <c r="C33" s="295"/>
@@ -19432,7 +19438,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="295" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B34" s="295"/>
       <c r="C34" s="295"/>
@@ -19445,7 +19451,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="295" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B35" s="295"/>
       <c r="C35" s="295"/>
@@ -19458,7 +19464,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="295" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B36" s="295"/>
       <c r="C36" s="295"/>
@@ -19471,7 +19477,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="295" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B37" s="295"/>
       <c r="C37" s="295"/>
@@ -19484,7 +19490,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="295" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B38" s="295"/>
       <c r="C38" s="295"/>
@@ -19497,7 +19503,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="295" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B39" s="295"/>
       <c r="C39" s="295"/>
@@ -19529,7 +19535,7 @@
       <c r="D41" s="295"/>
       <c r="E41" s="296"/>
       <c r="F41" s="342" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="G41" s="342"/>
       <c r="H41" s="342"/>
@@ -19542,7 +19548,7 @@
       <c r="D42" s="295"/>
       <c r="E42" s="296"/>
       <c r="F42" s="342" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="G42" s="342"/>
       <c r="H42" s="342"/>

</xml_diff>

<commit_message>
fix: Update price comparison JSON output with corrected values and additional divergences
</commit_message>
<xml_diff>
--- a/data/ORÇAMENTO - ACIONAMENTO 01 - REV 05 final.xlsx
+++ b/data/ORÇAMENTO - ACIONAMENTO 01 - REV 05 final.xlsx
@@ -6063,7 +6063,7 @@
     <t xml:space="preserve">DRIVER DE REPOSICAO PARA PLAFON DE LED EMBUTIR E SOBREPOR 36W</t>
   </si>
   <si>
-    <t xml:space="preserve"> 88264 </t>
+    <t xml:space="preserve"> 882645 </t>
   </si>
   <si>
     <t xml:space="preserve"> 95332 </t>
@@ -12183,7 +12183,7 @@
   <dimension ref="A1:L125"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>